<commit_message>
make participant ID compulsory add tips to excel sheet
</commit_message>
<xml_diff>
--- a/demographics.xlsx
+++ b/demographics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\44797\PycharmProjects\OSARI-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75F693D5-7A2D-4F4B-AC36-BA95BB66B396}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C30AFD42-2A51-4C6A-A5CB-20D30B078064}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{77476764-9DA6-44CA-8798-62768A9B6552}"/>
   </bookViews>
@@ -33,11 +33,44 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={41A1B9C5-6142-4A2F-80CB-050F01F30933}</author>
+    <author>tc={E965CDB6-2181-427E-B768-EAC3316FD164}</author>
+    <author>tc={8BDA48AE-73BF-445A-A54D-30E2F414335E}</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{41A1B9C5-6142-4A2F-80CB-050F01F30933}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Name of the field to present in the startup gui</t>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="1" shapeId="0" xr:uid="{E965CDB6-2181-427E-B768-EAC3316FD164}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    The default value to present in the startup gui</t>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="2" shapeId="0" xr:uid="{8BDA48AE-73BF-445A-A54D-30E2F414335E}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    The corresponding "tip" to be presented when the mouse hovers over this field in the startup gui</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
-  <si>
-    <t>Field</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Default</t>
   </si>
@@ -45,9 +78,6 @@
     <t>Age (Years)</t>
   </si>
   <si>
-    <t>Participan ID</t>
-  </si>
-  <si>
     <t>Gender</t>
   </si>
   <si>
@@ -63,9 +93,6 @@
     <t>Tip</t>
   </si>
   <si>
-    <t>Participant identifier</t>
-  </si>
-  <si>
     <t>Age in years</t>
   </si>
   <si>
@@ -73,13 +100,16 @@
   </si>
   <si>
     <t>The gender you identify as if non of the dropdown boxes are applicable</t>
+  </si>
+  <si>
+    <t>Name</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -87,13 +117,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -108,8 +150,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -125,6 +168,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Becca Hirst" id="{C8B08CA7-D946-402B-A23B-1CD9CE4F513B}" userId="Becca Hirst" providerId="None"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -422,47 +471,63 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="A1" dT="2021-07-05T19:09:20.40" personId="{C8B08CA7-D946-402B-A23B-1CD9CE4F513B}" id="{41A1B9C5-6142-4A2F-80CB-050F01F30933}">
+    <text>Name of the field to present in the startup gui</text>
+  </threadedComment>
+  <threadedComment ref="B1" dT="2021-07-05T19:09:39.50" personId="{C8B08CA7-D946-402B-A23B-1CD9CE4F513B}" id="{E965CDB6-2181-427E-B768-EAC3316FD164}">
+    <text>The default value to present in the startup gui</text>
+  </threadedComment>
+  <threadedComment ref="C1" dT="2021-07-05T19:10:01.16" personId="{C8B08CA7-D946-402B-A23B-1CD9CE4F513B}" id="{8BDA48AE-73BF-445A-A54D-30E2F414335E}">
+    <text>The corresponding "tip" to be presented when the mouse hovers over this field in the startup gui</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84CF4574-981F-4DDD-A0BB-78D77A63DF2C}">
-  <dimension ref="A1:C5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84CF4574-981F-4DDD-A0BB-78D77A63DF2C}">
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="28.08984375" customWidth="1"/>
+    <col min="2" max="2" width="49.26953125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>8</v>
+      <c r="C1" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3">
-        <v>0</v>
+      <c r="B3" t="s">
+        <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
@@ -473,22 +538,12 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>